<commit_message>
Data used to create visuals
</commit_message>
<xml_diff>
--- a/Tableau Tables/Tableau Table 1.xlsx
+++ b/Tableau Tables/Tableau Table 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Portfolio-Project-Covid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Portfolio-Project-Covid\Tableau Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B5D6D5-AA37-4F50-9426-69E6267B6C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40FFF20-50E7-49C5-8E8E-79E12A65116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{976A6CBF-2259-43E7-B902-9BFCA0BEC4F6}"/>
   </bookViews>
@@ -33,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>total_cases</t>
   </si>
   <si>
     <t>total_deaths</t>
-  </si>
-  <si>
-    <t>DeathPercentage</t>
   </si>
   <si>
     <t>total_vaccinations</t>
@@ -396,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EF2430-A64C-4F08-A10B-C99E72C4AA15}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,7 +407,7 @@
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,11 +417,8 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>389428321</v>
       </c>
@@ -432,9 +426,6 @@
         <v>5698368</v>
       </c>
       <c r="C2">
-        <v>1.4632000000000001</v>
-      </c>
-      <c r="D2">
         <v>10701388790</v>
       </c>
     </row>

</xml_diff>